<commit_message>
updating repo with most recent files and optimizatin trials
</commit_message>
<xml_diff>
--- a/IEA_15MW_semisub_files/IEA_15MW_semisub_output_comparisons.xlsx
+++ b/IEA_15MW_semisub_files/IEA_15MW_semisub_output_comparisons.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpotere\Documents\git\nrel_summer_2021\IEA_15MW_semisub_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65305232-555D-45D9-B948-9C4021343D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664187E5-476A-43BA-A306-2738C040FA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{191BF30B-01BE-4638-A576-71EAB7E0E6DB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{191BF30B-01BE-4638-A576-71EAB7E0E6DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="1" r:id="rId1"/>
     <sheet name="Optimization" sheetId="3" r:id="rId2"/>
+    <sheet name="fixed_ballast" sheetId="5" r:id="rId3"/>
+    <sheet name="hull_mass" sheetId="7" r:id="rId4"/>
+    <sheet name="displacement" sheetId="9" r:id="rId5"/>
+    <sheet name="variable_ballast" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="235">
   <si>
     <t>iea15mw_semisub.pdf metrics</t>
   </si>
@@ -754,21 +758,273 @@
     <t>set stress and global buckling back to False
 DV:members:main_col:diameter</t>
   </si>
+  <si>
+    <t>merit figure = floatingse.platform_ballast_mass</t>
+  </si>
+  <si>
+    <t>Initial DV = col1/2/3 ballast. Near optimality</t>
+  </si>
+  <si>
+    <t>Values Changed</t>
+  </si>
+  <si>
+    <t>added col1/2/3 diamater DV</t>
+  </si>
+  <si>
+    <t>SNOPT "optimal" changed from 1.3E-1 to 9.0E-2
+No change to diameter values</t>
+  </si>
+  <si>
+    <t>added col1/2/3 keel z-coordinate DV</t>
+  </si>
+  <si>
+    <t>SNOPT "optimal" changed from 9.0E-2 to 4.5E-1
+MeritFunction value is smaller though
+no change in z or diameter</t>
+  </si>
+  <si>
+    <t>added fixed_ballast_capacity constraint</t>
+  </si>
+  <si>
+    <t>SNOPT "optimal" changed from 4.5E-1 to 4.9E-1
+MeritFunction value is smaller though
+small changes in some sections of z and diameter values NOT significant</t>
+  </si>
+  <si>
+    <t>added col1/2/3 thickness DV</t>
+  </si>
+  <si>
+    <t>SNOPT "optimal" changed from 4.9E-1 to 4.2E-1
+MeritFunction value is larger
+small changes in some sections of z diameter and thickness values NOT significant</t>
+  </si>
+  <si>
+    <t>Initial DV = col1/2/3 keel z coordinates</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>added main_keel DV</t>
+  </si>
+  <si>
+    <t>Optimal = 5.8E-3
+Merit figure jumped from 3.65E-11 to 4.23E-11 mid run why?</t>
+  </si>
+  <si>
+    <t>removed main_keel DV
+added col1/2/3 diameter DV</t>
+  </si>
+  <si>
+    <t>Optimal = 8.4E-3, higher
+Merit figure = 7.47E-10, slight increases throughout run
+minor differences in values from base geometry</t>
+  </si>
+  <si>
+    <t>Optimal = 1.8E-3
+Merit figure is higher though, 4.085E-9….
+minor differences in values from base geometry</t>
+  </si>
+  <si>
+    <t>Optimal = 4.8E-2, larger than last run
+MeritFigure = 6.14E-7, significantly higher than last time
+minor differences in values from base geometry</t>
+  </si>
+  <si>
+    <t>merit figure = floatingse.platform_hull_mass</t>
+  </si>
+  <si>
+    <t>changed optimizer tol: 1e-6
+changed max_major iters: 50</t>
+  </si>
+  <si>
+    <t>no change in outputs or SNOPT files.</t>
+  </si>
+  <si>
+    <t>reverted changes in T5
+add col1/2/3 r_coord DV</t>
+  </si>
+  <si>
+    <t>Optimal= 4.7E-2, smaller than last
+MeritFigure= 6.32E-7
+Minor differences in values from base geometry</t>
+  </si>
+  <si>
+    <t>add main keel DV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MeritFigure= 6.45E-7, slightly higher
+</t>
+  </si>
+  <si>
+    <t>add main_column diameter and thickness DV</t>
+  </si>
+  <si>
+    <t>Optimal 5.2E-2
+MeritFigure=4.98E-7, smaller than last time
+minimal changes in values from base geometry</t>
+  </si>
+  <si>
+    <t>add pontoon_lower1/2/3 diameter DV</t>
+  </si>
+  <si>
+    <t>Otimal 5.3E-2
+MeritFigure= 4.895E-7
+minimal changes in values from base geometry</t>
+  </si>
+  <si>
+    <t>add pontoon_lower1/2/3 thickness DV</t>
+  </si>
+  <si>
+    <t>Optimal 7.2E-2
+MeritfFigure = 6.3E-9, improvement
+minimal changes in values from base geometry</t>
+  </si>
+  <si>
+    <t>add pontoon_upper1/2/3 diameter and thickness DV</t>
+  </si>
+  <si>
+    <t>Optimal 7.2E-2
+MeritFigure = 8.28E-11, improvement
+minimal changes in values from base geometry</t>
+  </si>
+  <si>
+    <t>add col1/2/3 diameter and thickness DV</t>
+  </si>
+  <si>
+    <t>Optimal = 5.8E-3
+MeritFigure = 2.21E-9
+No significant change in base geometry</t>
+  </si>
+  <si>
+    <t>Optimal = 1.7E-2
+MeritFigure = 7.6E-12
+No significant change in base geometry</t>
+  </si>
+  <si>
+    <t>add col1/2/3 r_coord DV</t>
+  </si>
+  <si>
+    <t>Optimal = 1.5E-2
+MeritFigure = 2.2E-9
+No significant change in base geometry</t>
+  </si>
+  <si>
+    <t>Optimal = 1.7E-2
+MeritFigure = 9.6E-9
+No significant change in base geometry</t>
+  </si>
+  <si>
+    <t>add main col keel DV</t>
+  </si>
+  <si>
+    <t>add main col diameter DV</t>
+  </si>
+  <si>
+    <t>remove main col diameter DV
+add main column thickness DV</t>
+  </si>
+  <si>
+    <t>ERROR on iteration 11</t>
+  </si>
+  <si>
+    <t>removed col1/2/3 and main col thickness DVs
+add pontoon_lower diameter DV</t>
+  </si>
+  <si>
+    <t>remove pontoon_lower diameter DV
+add pontoon_upper diameter DV</t>
+  </si>
+  <si>
+    <t>Optimal = 1.2E-2
+MeritFigure = 5.6E-9
+No significant change in base geometry
+how does this have an impact on displacement?</t>
+  </si>
+  <si>
+    <t>MeritFigure = 1.07E-10
+message that outer diameter has no impact on merit figure</t>
+  </si>
+  <si>
+    <t>ERROR on iteration 1
+note/message that outer diameter has no impact on merit figure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optimal = 1.0E-2
+MeritFigure = 4.7E-9
+col1/2/3 extended by 0.35 meters </t>
+  </si>
+  <si>
+    <t>add col1/2/3 diameter DV</t>
+  </si>
+  <si>
+    <t>Optimal = 2.3E-2
+MeritFigure = 6.19E-9
+small deviations from original design, max 0.13 meters in diameter change</t>
+  </si>
+  <si>
+    <t>add r_coord col1/2/3</t>
+  </si>
+  <si>
+    <t>Optimal = 2.9E-2
+MeritFigure =4.5E-10
+minimal deviation original geometry</t>
+  </si>
+  <si>
+    <t>add col1/2/3 thickness DV</t>
+  </si>
+  <si>
+    <t>Optimal = 2.9E-2
+MeritFigure =1.09E-7
+minimal deviation original geometry</t>
+  </si>
+  <si>
+    <t>add main_keel DV</t>
+  </si>
+  <si>
+    <t>Optimal = 2.9E-2
+MeritFigure = 2.5E-9
+minimal deviation original geometry</t>
+  </si>
+  <si>
+    <t>add variable_ballast_capacity constraint</t>
+  </si>
+  <si>
+    <t>ERROR: same as before</t>
+  </si>
+  <si>
+    <t>remove variable_ballast_capacity constraint
+add main_column diameter DV</t>
+  </si>
+  <si>
+    <t>Optimal = 2.9E-2
+MeritFigure = 4.4E-8
+minimal deviation original geometry</t>
+  </si>
+  <si>
+    <t>add main_column thickness DV</t>
+  </si>
+  <si>
+    <t>Optimal = 2.9E-2
+MeritFigure = 1.8E-7
+minimal deviation original geometry</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="166" formatCode="0.000000E+00"/>
-    <numFmt numFmtId="167" formatCode="0.0000000E+00"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.000000000000E+00"/>
-    <numFmt numFmtId="171" formatCode="0.00000000E+00"/>
-    <numFmt numFmtId="175" formatCode="0.0000000000000E+00"/>
-    <numFmt numFmtId="176" formatCode="0.00000000000000E+00"/>
-    <numFmt numFmtId="180" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000000E+00"/>
+    <numFmt numFmtId="169" formatCode="0.00000000E+00"/>
+    <numFmt numFmtId="170" formatCode="0.0000000000000E+00"/>
+    <numFmt numFmtId="171" formatCode="0.00000000000000E+00"/>
+    <numFmt numFmtId="172" formatCode="0.0000"/>
+    <numFmt numFmtId="173" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -825,34 +1081,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,7 +1428,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
@@ -1459,11 +1717,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A4121F8-F02A-4549-8E5C-4B8B9995F331}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M43" sqref="M43"/>
+      <selection pane="bottomRight" sqref="A1:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3646,4 +3904,1166 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B85ED78-0BF9-4FF1-8EE4-7793BA760DB3}">
+  <dimension ref="A1:O8"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="11" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" style="12" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.36328125" style="12" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="42.08984375" style="15" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="38.26953125" style="15" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="33.90625" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="12" width="29.453125" style="10" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="71" customWidth="1"/>
+    <col min="15" max="15" width="127.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <v>17854000</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3914000</v>
+      </c>
+      <c r="E3" s="11">
+        <v>2540000</v>
+      </c>
+      <c r="F3" s="12">
+        <v>11300000</v>
+      </c>
+      <c r="G3" s="15">
+        <v>-13.63</v>
+      </c>
+      <c r="H3" s="15">
+        <v>-14.94</v>
+      </c>
+      <c r="I3" s="4">
+        <v>20206</v>
+      </c>
+      <c r="J3" s="10">
+        <v>12510000000</v>
+      </c>
+      <c r="K3" s="10">
+        <v>12510000000</v>
+      </c>
+      <c r="L3" s="10">
+        <v>23670000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="11">
+        <v>2539999.9945295001</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2539999.9938535602</v>
+      </c>
+      <c r="M5" t="s">
+        <v>174</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="11">
+        <v>2539999.99922485</v>
+      </c>
+      <c r="M6" t="s">
+        <v>176</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="11">
+        <v>2539999.9999494501</v>
+      </c>
+      <c r="M7" t="s">
+        <v>178</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="11">
+        <v>2539999.9988705199</v>
+      </c>
+      <c r="M8" t="s">
+        <v>180</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0AB80C-1E1B-4F6B-BD4E-44B3DAA5D4D6}">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="11" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" style="12" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="33.6328125" style="11" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="33.36328125" style="12" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="42.08984375" style="15" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="38.26953125" style="15" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="33.90625" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="12" width="29.453125" style="10" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="42.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="71" customWidth="1"/>
+    <col min="15" max="15" width="127.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <v>17854000</v>
+      </c>
+      <c r="D3" s="12">
+        <v>3914000</v>
+      </c>
+      <c r="E3" s="11">
+        <v>2540000</v>
+      </c>
+      <c r="F3" s="12">
+        <v>11300000</v>
+      </c>
+      <c r="G3" s="15">
+        <v>-13.63</v>
+      </c>
+      <c r="H3" s="15">
+        <v>-14.94</v>
+      </c>
+      <c r="I3" s="4">
+        <v>20206</v>
+      </c>
+      <c r="J3" s="10">
+        <v>12510000000</v>
+      </c>
+      <c r="K3" s="10">
+        <v>12510000000</v>
+      </c>
+      <c r="L3" s="10">
+        <v>23670000000</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="12">
+        <v>3914000.0001656101</v>
+      </c>
+      <c r="M4" t="s">
+        <v>183</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="12">
+        <v>3914000.0159891001</v>
+      </c>
+      <c r="M5" t="s">
+        <v>184</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="12">
+        <v>3914000.0029250002</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="12">
+        <v>3913997.5943076299</v>
+      </c>
+      <c r="M7" t="s">
+        <v>180</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="12">
+        <v>3913997.5242918101</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="12">
+        <v>3913997.4742234498</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="12">
+        <v>3913998.0501684202</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="12">
+        <v>3913998.0840118402</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="12">
+        <v>3913999.9753387002</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="12">
+        <v>3913999.99967568</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F00F0C-E96F-4EB2-8A1F-74DF6101BCB2}">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="11" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" style="12" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" style="12" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.6328125" style="11" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="33.36328125" style="12" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="42.08984375" style="15" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="38.26953125" style="15" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="33.90625" style="23" customWidth="1"/>
+    <col min="10" max="12" width="29.453125" style="10" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="42.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="71" customWidth="1"/>
+    <col min="15" max="15" width="127.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <v>17854000</v>
+      </c>
+      <c r="D3" s="12">
+        <v>3914000</v>
+      </c>
+      <c r="E3" s="11">
+        <v>2540000</v>
+      </c>
+      <c r="F3" s="12">
+        <v>11300000</v>
+      </c>
+      <c r="G3" s="15">
+        <v>-13.63</v>
+      </c>
+      <c r="H3" s="15">
+        <v>-14.94</v>
+      </c>
+      <c r="I3" s="23">
+        <v>20206</v>
+      </c>
+      <c r="J3" s="10">
+        <v>12510000000</v>
+      </c>
+      <c r="K3" s="10">
+        <v>12510000000</v>
+      </c>
+      <c r="L3" s="10">
+        <v>23670000000</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="12">
+        <v>3914000.0001656101</v>
+      </c>
+      <c r="I4" s="23">
+        <v>20206.00004472</v>
+      </c>
+      <c r="M4" t="s">
+        <v>183</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="12">
+        <v>3914000.0159891001</v>
+      </c>
+      <c r="I5" s="23">
+        <v>20205.999999849999</v>
+      </c>
+      <c r="M5" t="s">
+        <v>205</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="12">
+        <v>3914000.0029250002</v>
+      </c>
+      <c r="I6" s="23">
+        <v>20205.99995383</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="12">
+        <v>3913997.5943076299</v>
+      </c>
+      <c r="I7" s="23">
+        <v>20205.999999799998</v>
+      </c>
+      <c r="M7" t="s">
+        <v>211</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" t="s">
+        <v>212</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="12">
+        <v>3913997.5242918101</v>
+      </c>
+      <c r="I9" s="23">
+        <v>20205.999886559999</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="12">
+        <v>3913997.4742234498</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="12">
+        <v>3913998.0501684202</v>
+      </c>
+      <c r="I11" s="23">
+        <v>20205.999997819999</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="12">
+        <v>3913998.0840118402</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="12">
+        <v>3913999.9753387002</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="12">
+        <v>3913999.99967568</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EDC2461-B9B5-4D0B-8807-3ADBAA558556}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="11" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" style="12" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" style="12" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.6328125" style="11" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="33.36328125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="42.08984375" style="15" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="38.26953125" style="15" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="33.90625" style="23" hidden="1" customWidth="1"/>
+    <col min="10" max="12" width="29.453125" style="10" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="42.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="71" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <v>17854000</v>
+      </c>
+      <c r="D3" s="12">
+        <v>3914000</v>
+      </c>
+      <c r="E3" s="11">
+        <v>2540000</v>
+      </c>
+      <c r="F3" s="12">
+        <v>11300000</v>
+      </c>
+      <c r="G3" s="15">
+        <v>-13.63</v>
+      </c>
+      <c r="H3" s="15">
+        <v>-14.94</v>
+      </c>
+      <c r="I3" s="23">
+        <v>20206</v>
+      </c>
+      <c r="J3" s="10">
+        <v>12510000000</v>
+      </c>
+      <c r="K3" s="10">
+        <v>12510000000</v>
+      </c>
+      <c r="L3" s="10">
+        <v>23670000000</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="12">
+        <v>3914000.0001656101</v>
+      </c>
+      <c r="F4" s="12">
+        <v>11300000.0531576</v>
+      </c>
+      <c r="I4" s="23">
+        <v>20206.00004472</v>
+      </c>
+      <c r="M4" t="s">
+        <v>183</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="12">
+        <v>3914000.0159891001</v>
+      </c>
+      <c r="F5" s="12">
+        <v>11299999.9299748</v>
+      </c>
+      <c r="I5" s="23">
+        <v>20205.999999849999</v>
+      </c>
+      <c r="M5" t="s">
+        <v>221</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="12">
+        <v>3914000.0029250002</v>
+      </c>
+      <c r="F6" s="12">
+        <v>11299999.994837301</v>
+      </c>
+      <c r="I6" s="23">
+        <v>20205.99995383</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="12">
+        <v>3913997.5943076299</v>
+      </c>
+      <c r="F7" s="12">
+        <v>11300001.240620701</v>
+      </c>
+      <c r="I7" s="23">
+        <v>20205.999999799998</v>
+      </c>
+      <c r="M7" t="s">
+        <v>225</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="12">
+        <v>11300000.028921699</v>
+      </c>
+      <c r="M8" t="s">
+        <v>227</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="12">
+        <v>3913997.5242918101</v>
+      </c>
+      <c r="I9" s="23">
+        <v>20205.999886559999</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="12">
+        <v>3913997.4742234498</v>
+      </c>
+      <c r="F10" s="12">
+        <v>11300000.501181999</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="12">
+        <v>3913998.0501684202</v>
+      </c>
+      <c r="F11" s="12">
+        <v>11300002.088639701</v>
+      </c>
+      <c r="I11" s="23">
+        <v>20205.999997819999</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="12">
+        <v>3913998.0840118402</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="12">
+        <v>3913999.9753387002</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="12">
+        <v>3913999.99967568</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>